<commit_message>
Completed my task for add user.
</commit_message>
<xml_diff>
--- a/com.hybridframework.orangehrm.project01/testdata/data.xlsx
+++ b/com.hybridframework.orangehrm.project01/testdata/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13590" windowHeight="6615" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,13 @@
     <sheet name="Sachin" sheetId="6" r:id="rId6"/>
     <sheet name="Anita" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -36,12 +37,33 @@
   <si>
     <t>admin234</t>
   </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Hodo5613</t>
+  </si>
+  <si>
+    <t>hodo0219</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,15 +72,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -66,19 +94,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -157,6 +207,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -191,6 +242,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -366,20 +418,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -387,7 +439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -395,7 +447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -409,76 +461,113 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>